<commit_message>
Adapt test file to use a segmentation with namespace.
Currently, a "tok" column would also be outputted as namespaced segmentation instead of using it  as the base token layer.
</commit_message>
<xml_diff>
--- a/tests/data/import/xlsx/sample_sentence_with_namespace/doc1.xlsx
+++ b/tests/data/import/xlsx/sample_sentence_with_namespace/doc1.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t xml:space="preserve">tok</t>
+    <t xml:space="preserve">default_ns::text</t>
   </si>
   <si>
     <t xml:space="preserve">mynamespace::lb</t>
@@ -276,11 +276,12 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.33"/>
   </cols>
   <sheetData>

</xml_diff>